<commit_message>
Added 10 second wait time for each site to load.
</commit_message>
<xml_diff>
--- a/price_extractor.xlsx
+++ b/price_extractor.xlsx
@@ -475,12 +475,12 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Not found</t>
+          <t>That's Smart! Fat Free Skim Milk</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Not found</t>
+          <t>$2.72</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Several attempts to fix Walmart issue.
</commit_message>
<xml_diff>
--- a/price_extractor.xlsx
+++ b/price_extractor.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C20"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -463,7 +463,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>2.839</t>
+          <t>2.689</t>
         </is>
       </c>
     </row>
@@ -475,12 +475,12 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Not found</t>
+          <t>That's Smart! Fat Free Skim Milk</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Not found</t>
+          <t>$2.72</t>
         </is>
       </c>
     </row>
@@ -517,253 +517,6 @@
           <t>Not found</t>
         </is>
       </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>https://www.walmart.com/ip/Sara-Lee-Artesano-Brioche-Hamburger-Buns-8-count-16-oz/602085634</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Not found</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Not found</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>https://www.walmart.com/ip/Great-Value-Mayonnaise-30-fl-oz/17056888</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>Not found</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>Not found</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>https://www.walmart.com/ip/Great-Value-Pear-Halves-in-Pear-Juice-15-oz/10415589</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>Not found</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>Not found</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>https://www.walmart.com/ip/Fresh-Romaine-Lettuce-Hearts-3-Count-Each/10532755</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>Not found</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>Not found</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>https://www.walmart.com/ip/Great-Value-Thin-Sliced-Oven-Roasted-Turkey-Breast-Family-Pack-16-oz-Plastic-Tub-9-Grams-of-Protein-per-2-oz-Serving/47394316</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>Not found</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>Not found</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>https://www.walmart.com/ip/Great-Value-4-Milkfat-Minimum-Small-Curd-Cottage-Cheese-24-oz/10315022</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>Not found</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>Not found</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>https://www.walmart.com/ip/Fairlife-Fat-Free-Ultra-Filtered-Milk-52-fl-oz/43984342</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>Not found</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>Not found</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>https://www.walmart.com/ip/Fresh-Banana-Fruit-Each/44390948</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>Not found</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>Not found</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>https://www.walmart.com/ip/Clementines-3-lbs/11025598</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>Not found</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>Not found</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>https://www.hy-vee.com/aisles-online/p/31823/Certified-Ground-Round-90-Lean-10-Fat</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>Certified Ground Round 90% Lean 10% Fat</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr"/>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>https://www.hy-vee.com/aisles-online/p/65791/Boneless-Skinless-Chicken-Breast</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>Not found</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>Not found</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>https://www.ramtrucks.com/ram-1500.html</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>2025 Ram 1500</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>$40,275</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>https://www.chevrolet.com/trucks/silverado/1500</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>Not found</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>Not found</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>https://www.menards.com/main/building-materials/lumber-boards/dimensional-lumber/2-x-4-construction-framing-lumber/1021101/p-1444451086852-c-13125.htm</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>Not found</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>Not found</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>https://www.hy-vee.com/aisles-online/p/22365/HyVee-Select-100-Pure-Maple-Syrup</t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>Hy-Vee Select 100% Pure Maple Syrup</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Pushed automatic run and merged Excel file
</commit_message>
<xml_diff>
--- a/price_extractor.xlsx
+++ b/price_extractor.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C23"/>
+  <dimension ref="A1:O23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -449,6 +449,66 @@
           <t>Price</t>
         </is>
       </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Product Name.1</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Price.1</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Product Name.2</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Price.2</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Product Name.3</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Price.3</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Product Name_2025-02-12 14:57</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Price_2025-02-12 14:57</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>Product Name_2025-02-14 03:04</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Price_2025-02-14 03:04</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>Product Name_2025-02-14 08:31</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>Price_2025-02-14 08:31</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -463,7 +523,67 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
+          <t>2.949</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>UNLEADED 87 (10% ETH)</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>2.779</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>UNLEADED 87 (10% ETH)</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
           <t>2.729</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>UNLEADED 87 (10% ETH)</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>2.729</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>UNLEADED 87 (10% ETH)</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>2.729</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>UNLEADED 87 (10% ETH)</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>2.999</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>UNLEADED 87 (10% ETH)</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>2.999</t>
         </is>
       </c>
     </row>
@@ -483,6 +603,66 @@
           <t>$2.72</t>
         </is>
       </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>That's Smart! Fat Free Skim Milk</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>$2.72</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>That's Smart! Fat Free Skim Milk</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>$2.72</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>That's Smart! Fat Free Skim Milk</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>$2.72</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>That's Smart! Fat Free Skim Milk</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>$2.72</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>That's Smart! Fat Free Skim Milk</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>$2.72</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>That's Smart! Fat Free Skim Milk</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>$2.72</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -500,6 +680,66 @@
           <t>32¢ ea.</t>
         </is>
       </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Roma Tomatoes</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>32¢ ea.</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Roma Tomatoes</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>32¢ ea.</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>Roma Tomatoes</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>32¢ ea.</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>Roma Tomatoes</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>32¢ ea.</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>Roma Tomatoes</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>32¢ ea.</t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>Roma Tomatoes</t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>32¢ ea.</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -517,6 +757,66 @@
           <t>$4.97</t>
         </is>
       </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Quaker Cap'n Crunch Regular Cereal</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>$4.97</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Quaker Cap'n Crunch Regular Cereal</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>$4.97</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>Quaker Cap'n Crunch Regular Cereal</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>$4.97</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>Quaker Cap'n Crunch Regular Cereal</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>$4.97</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>Quaker Cap'n Crunch Regular Cereal</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>$4.97</t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>Quaker Cap'n Crunch Regular Cereal</t>
+        </is>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>$4.97</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -534,6 +834,66 @@
           <t>$3.99</t>
         </is>
       </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Sara Lee Artesano Brioche Buns, 8 count</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>$3.99</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>Sara Lee Artesano Brioche Buns, 8 count</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>$3.99</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>Sara Lee Artesano Brioche Buns, 8 count</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>$3.99</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>Sara Lee Artesano Brioche Buns, 8 count</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>$3.99</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>Sara Lee Artesano Brioche Buns, 8 count</t>
+        </is>
+      </c>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>$3.99</t>
+        </is>
+      </c>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>Sara Lee Artesano Brioche Buns, 8 count</t>
+        </is>
+      </c>
+      <c r="O6" t="inlineStr">
+        <is>
+          <t>$3.99</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -551,6 +911,66 @@
           <t>$3.65</t>
         </is>
       </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>That's Smart! Mayonnaise</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>$3.65</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>That's Smart! Mayonnaise</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>$3.65</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>That's Smart! Mayonnaise</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>$3.65</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>That's Smart! Mayonnaise</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>$3.65</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>That's Smart! Mayonnaise</t>
+        </is>
+      </c>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>$3.65</t>
+        </is>
+      </c>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t>That's Smart! Mayonnaise</t>
+        </is>
+      </c>
+      <c r="O7" t="inlineStr">
+        <is>
+          <t>$3.65</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -568,6 +988,66 @@
           <t>$1.99</t>
         </is>
       </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Hy-Vee Light Bartlett Pear Halves In Pear Juice From Concentrate</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>$1.99</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>Hy-Vee Light Bartlett Pear Halves In Pear Juice From Concentrate</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>$1.99</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>Hy-Vee Light Bartlett Pear Halves In Pear Juice From Concentrate</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>$1.99</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>Hy-Vee Light Bartlett Pear Halves In Pear Juice From Concentrate</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>$1.99</t>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>Hy-Vee Light Bartlett Pear Halves In Pear Juice From Concentrate</t>
+        </is>
+      </c>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>$1.99</t>
+        </is>
+      </c>
+      <c r="N8" t="inlineStr">
+        <is>
+          <t>Hy-Vee Light Bartlett Pear Halves In Pear Juice From Concentrate</t>
+        </is>
+      </c>
+      <c r="O8" t="inlineStr">
+        <is>
+          <t>$1.99</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -582,6 +1062,66 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
+          <t>$3.99</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Dole Fresh Romaine Hearts</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>$3.69</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>Dole Fresh Romaine Hearts</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>$3.69</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>Dole Fresh Romaine Hearts</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>$3.69</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>Dole Fresh Romaine Hearts</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>$3.69</t>
+        </is>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>Dole Fresh Romaine Hearts</t>
+        </is>
+      </c>
+      <c r="M9" t="inlineStr">
+        <is>
+          <t>$3.69</t>
+        </is>
+      </c>
+      <c r="N9" t="inlineStr">
+        <is>
+          <t>Dole Fresh Romaine Hearts</t>
+        </is>
+      </c>
+      <c r="O9" t="inlineStr">
+        <is>
           <t>$3.69</t>
         </is>
       </c>
@@ -602,6 +1142,66 @@
           <t>$5.79</t>
         </is>
       </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Hy-Vee Oven Roasted Cured Turkey Breast &amp; White Turkey Shaved Slices</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>$5.79</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>Hy-Vee Oven Roasted Cured Turkey Breast &amp; White Turkey Shaved Slices</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>$5.79</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>Hy-Vee Oven Roasted Cured Turkey Breast &amp; White Turkey Shaved Slices</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>$5.79</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>Hy-Vee Oven Roasted Cured Turkey Breast &amp; White Turkey Shaved Slices</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>$5.79</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>Hy-Vee Oven Roasted Cured Turkey Breast &amp; White Turkey Shaved Slices</t>
+        </is>
+      </c>
+      <c r="M10" t="inlineStr">
+        <is>
+          <t>$5.79</t>
+        </is>
+      </c>
+      <c r="N10" t="inlineStr">
+        <is>
+          <t>Hy-Vee Oven Roasted Cured Turkey Breast &amp; White Turkey Shaved Slices</t>
+        </is>
+      </c>
+      <c r="O10" t="inlineStr">
+        <is>
+          <t>$5.79</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -619,6 +1219,66 @@
           <t>$2.99</t>
         </is>
       </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>That's Smart! Small Curd Cottage Cheese 4% Milkfat</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>$2.99</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>That's Smart! Small Curd Cottage Cheese 4% Milkfat</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>$2.99</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>That's Smart! Small Curd Cottage Cheese 4% Milkfat</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>$2.99</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>That's Smart! Small Curd Cottage Cheese 4% Milkfat</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>$2.99</t>
+        </is>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>That's Smart! Small Curd Cottage Cheese 4% Milkfat</t>
+        </is>
+      </c>
+      <c r="M11" t="inlineStr">
+        <is>
+          <t>$2.99</t>
+        </is>
+      </c>
+      <c r="N11" t="inlineStr">
+        <is>
+          <t>That's Smart! Small Curd Cottage Cheese 4% Milkfat</t>
+        </is>
+      </c>
+      <c r="O11" t="inlineStr">
+        <is>
+          <t>$2.99</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -636,6 +1296,66 @@
           <t>$4.97</t>
         </is>
       </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Fairlife Fat Free Ultra-Filtered Milk</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>$4.97</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>Fairlife Fat Free Ultra-Filtered Milk</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>$4.97</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>Fairlife Fat Free Ultra-Filtered Milk</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>$4.97</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>Fairlife Fat Free Ultra-Filtered Milk</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>$4.97</t>
+        </is>
+      </c>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>Fairlife Fat Free Ultra-Filtered Milk</t>
+        </is>
+      </c>
+      <c r="M12" t="inlineStr">
+        <is>
+          <t>$4.97</t>
+        </is>
+      </c>
+      <c r="N12" t="inlineStr">
+        <is>
+          <t>Fairlife Fat Free Ultra-Filtered Milk</t>
+        </is>
+      </c>
+      <c r="O12" t="inlineStr">
+        <is>
+          <t>$4.97</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -653,6 +1373,66 @@
           <t>16¢ ea.</t>
         </is>
       </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Fresh Chiquita Bananas</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>16¢ ea.</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>Fresh Chiquita Bananas</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>16¢ ea.</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>Fresh Chiquita Bananas</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>16¢ ea.</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>Fresh Chiquita Bananas</t>
+        </is>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>16¢ ea.</t>
+        </is>
+      </c>
+      <c r="L13" t="inlineStr">
+        <is>
+          <t>Fresh Chiquita Bananas</t>
+        </is>
+      </c>
+      <c r="M13" t="inlineStr">
+        <is>
+          <t>16¢ ea.</t>
+        </is>
+      </c>
+      <c r="N13" t="inlineStr">
+        <is>
+          <t>Fresh Chiquita Bananas</t>
+        </is>
+      </c>
+      <c r="O13" t="inlineStr">
+        <is>
+          <t>16¢ ea.</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -670,6 +1450,66 @@
           <t>$5.79</t>
         </is>
       </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Wonderful Halos Mandarin Oranges</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>$5.79</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>Wonderful Halos Mandarin Oranges</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>$5.79</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>Wonderful Halos Mandarin Oranges</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>$5.79</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>Wonderful Halos Mandarin Oranges</t>
+        </is>
+      </c>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>$5.79</t>
+        </is>
+      </c>
+      <c r="L14" t="inlineStr">
+        <is>
+          <t>Wonderful Halos Mandarin Oranges</t>
+        </is>
+      </c>
+      <c r="M14" t="inlineStr">
+        <is>
+          <t>$5.79</t>
+        </is>
+      </c>
+      <c r="N14" t="inlineStr">
+        <is>
+          <t>Wonderful Halos Mandarin Oranges</t>
+        </is>
+      </c>
+      <c r="O14" t="inlineStr">
+        <is>
+          <t>$5.79</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -687,6 +1527,66 @@
           <t>$6.99/lb</t>
         </is>
       </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>Certified Ground Round 90% Lean 10% Fat</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>$6.99/lb</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>Certified Ground Round 90% Lean 10% Fat</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>$6.99/lb</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>Certified Ground Round 90% Lean 10% Fat</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>$6.99/lb</t>
+        </is>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>Certified Ground Round 90% Lean 10% Fat</t>
+        </is>
+      </c>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t>$6.99/lb</t>
+        </is>
+      </c>
+      <c r="L15" t="inlineStr">
+        <is>
+          <t>Certified Ground Round 90% Lean 10% Fat</t>
+        </is>
+      </c>
+      <c r="M15" t="inlineStr">
+        <is>
+          <t>$6.99/lb</t>
+        </is>
+      </c>
+      <c r="N15" t="inlineStr">
+        <is>
+          <t>Certified Ground Round 90% Lean 10% Fat</t>
+        </is>
+      </c>
+      <c r="O15" t="inlineStr">
+        <is>
+          <t>$6.99/lb</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -704,6 +1604,66 @@
           <t>$4.07 ea.</t>
         </is>
       </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>Boneless Skinless Chicken Breast</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>$4.07 ea.</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>Boneless Skinless Chicken Breast</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>$4.07 ea.</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>Boneless Skinless Chicken Breast</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>$4.07 ea.</t>
+        </is>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>Boneless Skinless Chicken Breast</t>
+        </is>
+      </c>
+      <c r="K16" t="inlineStr">
+        <is>
+          <t>$4.07 ea.</t>
+        </is>
+      </c>
+      <c r="L16" t="inlineStr">
+        <is>
+          <t>Boneless Skinless Chicken Breast</t>
+        </is>
+      </c>
+      <c r="M16" t="inlineStr">
+        <is>
+          <t>$4.07 ea.</t>
+        </is>
+      </c>
+      <c r="N16" t="inlineStr">
+        <is>
+          <t>Boneless Skinless Chicken Breast</t>
+        </is>
+      </c>
+      <c r="O16" t="inlineStr">
+        <is>
+          <t>$4.07 ea.</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -721,6 +1681,66 @@
           <t>$40,275</t>
         </is>
       </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>2025 Ram 1500</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>$40,275</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>2025 Ram 1500</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>$40,275</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>2025 Ram 1500</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>$40,275</t>
+        </is>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>2025 Ram 1500</t>
+        </is>
+      </c>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t>$40,275</t>
+        </is>
+      </c>
+      <c r="L17" t="inlineStr">
+        <is>
+          <t>2025 Ram 1500</t>
+        </is>
+      </c>
+      <c r="M17" t="inlineStr">
+        <is>
+          <t>$40,275</t>
+        </is>
+      </c>
+      <c r="N17" t="inlineStr">
+        <is>
+          <t>2025 Ram 1500</t>
+        </is>
+      </c>
+      <c r="O17" t="inlineStr">
+        <is>
+          <t>$40,275</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -734,6 +1754,42 @@
           <t>$37,000*</t>
         </is>
       </c>
+      <c r="D18" t="inlineStr"/>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>$37,000*</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr"/>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>$37,000*</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr"/>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>$37,000*</t>
+        </is>
+      </c>
+      <c r="J18" t="inlineStr"/>
+      <c r="K18" t="inlineStr">
+        <is>
+          <t>$37,000*</t>
+        </is>
+      </c>
+      <c r="L18" t="inlineStr"/>
+      <c r="M18" t="inlineStr">
+        <is>
+          <t>$37,000*</t>
+        </is>
+      </c>
+      <c r="N18" t="inlineStr"/>
+      <c r="O18" t="inlineStr">
+        <is>
+          <t>$37,000*</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -741,11 +1797,7 @@
           <t>https://www.menards.com/main/building-materials/lumber-boards/dimensional-lumber/2-x-4-construction-framing-lumber/1021101/p-1444451086852-c-13125.htm</t>
         </is>
       </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>Not found</t>
-        </is>
-      </c>
+      <c r="B19" t="inlineStr"/>
       <c r="C19" t="inlineStr">
         <is>
           <t>$
@@ -754,6 +1806,64 @@
 each</t>
         </is>
       </c>
+      <c r="D19" t="inlineStr"/>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>$
+3
+85
+each</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr"/>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>$
+3
+85
+each</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>Not found</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>$
+3
+85
+each</t>
+        </is>
+      </c>
+      <c r="J19" t="inlineStr"/>
+      <c r="K19" t="inlineStr">
+        <is>
+          <t>$
+3
+85
+each</t>
+        </is>
+      </c>
+      <c r="L19" t="inlineStr"/>
+      <c r="M19" t="inlineStr">
+        <is>
+          <t>$
+3
+85
+each</t>
+        </is>
+      </c>
+      <c r="N19" t="inlineStr"/>
+      <c r="O19" t="inlineStr">
+        <is>
+          <t>$
+3
+85
+each</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -771,6 +1881,66 @@
           <t>$6.99</t>
         </is>
       </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>Hy-Vee Select 100% Pure Maple Syrup</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>$6.99</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>Hy-Vee Select 100% Pure Maple Syrup</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>$6.99</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>Hy-Vee Select 100% Pure Maple Syrup</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>$6.99</t>
+        </is>
+      </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>Hy-Vee Select 100% Pure Maple Syrup</t>
+        </is>
+      </c>
+      <c r="K20" t="inlineStr">
+        <is>
+          <t>$6.99</t>
+        </is>
+      </c>
+      <c r="L20" t="inlineStr">
+        <is>
+          <t>Hy-Vee Select 100% Pure Maple Syrup</t>
+        </is>
+      </c>
+      <c r="M20" t="inlineStr">
+        <is>
+          <t>$6.99</t>
+        </is>
+      </c>
+      <c r="N20" t="inlineStr">
+        <is>
+          <t>Hy-Vee Select 100% Pure Maple Syrup</t>
+        </is>
+      </c>
+      <c r="O20" t="inlineStr">
+        <is>
+          <t>$6.99</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -788,6 +1958,66 @@
           <t>$5.46</t>
         </is>
       </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>That's Smart! Large Shell Eggs</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>$5.46</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>That's Smart! Large Shell Eggs</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>$5.46</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>That's Smart! Large Shell Eggs</t>
+        </is>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>$5.46</t>
+        </is>
+      </c>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>That's Smart! Large Shell Eggs</t>
+        </is>
+      </c>
+      <c r="K21" t="inlineStr">
+        <is>
+          <t>$5.46</t>
+        </is>
+      </c>
+      <c r="L21" t="inlineStr">
+        <is>
+          <t>That's Smart! Large Shell Eggs</t>
+        </is>
+      </c>
+      <c r="M21" t="inlineStr">
+        <is>
+          <t>$5.46</t>
+        </is>
+      </c>
+      <c r="N21" t="inlineStr">
+        <is>
+          <t>That's Smart! Large Shell Eggs</t>
+        </is>
+      </c>
+      <c r="O21" t="inlineStr">
+        <is>
+          <t>$5.46</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -805,6 +2035,66 @@
           <t>698</t>
         </is>
       </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>5.5 cu.ft. Extra-Large Capacity Smart Top Load Washer with Super Speed in White</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>698</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>Not found</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>698</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>5.5 cu.ft. Extra-Large Capacity Smart Top Load Washer with Super Speed in White</t>
+        </is>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>698</t>
+        </is>
+      </c>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t>5.5 cu.ft. Extra-Large Capacity Smart Top Load Washer with Super Speed in White</t>
+        </is>
+      </c>
+      <c r="K22" t="inlineStr">
+        <is>
+          <t>698</t>
+        </is>
+      </c>
+      <c r="L22" t="inlineStr">
+        <is>
+          <t>Not found</t>
+        </is>
+      </c>
+      <c r="M22" t="inlineStr">
+        <is>
+          <t>698</t>
+        </is>
+      </c>
+      <c r="N22" t="inlineStr">
+        <is>
+          <t>Not found</t>
+        </is>
+      </c>
+      <c r="O22" t="inlineStr">
+        <is>
+          <t>698</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -818,6 +2108,66 @@
         </is>
       </c>
       <c r="C23" t="inlineStr">
+        <is>
+          <t>698</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>7.4 cu. ft. Vented Smart Front Load Electric Dryer with Steam Sanitize+ in White</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>698</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>Not found</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>698</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>7.4 cu. ft. Vented Smart Front Load Electric Dryer with Steam Sanitize+ in White</t>
+        </is>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>698</t>
+        </is>
+      </c>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t>7.4 cu. ft. Vented Smart Front Load Electric Dryer with Steam Sanitize+ in White</t>
+        </is>
+      </c>
+      <c r="K23" t="inlineStr">
+        <is>
+          <t>698</t>
+        </is>
+      </c>
+      <c r="L23" t="inlineStr">
+        <is>
+          <t>Not found</t>
+        </is>
+      </c>
+      <c r="M23" t="inlineStr">
+        <is>
+          <t>698</t>
+        </is>
+      </c>
+      <c r="N23" t="inlineStr">
+        <is>
+          <t>Not found</t>
+        </is>
+      </c>
+      <c r="O23" t="inlineStr">
         <is>
           <t>698</t>
         </is>

</xml_diff>